<commit_message>
update generator data to NETL data
</commit_message>
<xml_diff>
--- a/generator/fixOM.xlsx
+++ b/generator/fixOM.xlsx
@@ -1,23 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10510"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/canli/euler/work/GETP/generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3008A796-33FB-3B40-A283-003A102FED59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="38200" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="39380" yWindow="6320" windowWidth="38200" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Year</t>
   </si>
@@ -60,12 +69,15 @@
   </si>
   <si>
     <t>old</t>
+  </si>
+  <si>
+    <t>ratio from ES-4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -108,6 +120,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -375,15 +390,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -425,31 +441,33 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>59290</v>
+        <f>C2*B5</f>
+        <v>95360</v>
       </c>
       <c r="C2" s="2">
-        <v>40410</v>
+        <v>64000</v>
       </c>
       <c r="D2" s="2">
         <v>85030</v>
       </c>
       <c r="E2" s="2">
-        <v>27480</v>
+        <f>F2*E5</f>
+        <v>31070</v>
       </c>
       <c r="F2" s="2">
-        <v>14040</v>
+        <v>13000</v>
       </c>
       <c r="G2" s="2">
-        <v>6970</v>
+        <v>10000</v>
       </c>
       <c r="H2" s="2">
-        <v>121130</v>
+        <v>124000</v>
       </c>
       <c r="I2" s="2">
-        <v>15190</v>
+        <v>16000</v>
       </c>
       <c r="J2" s="2">
-        <v>26220</v>
+        <v>38000</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -495,6 +513,17 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>1.49</v>
+      </c>
+      <c r="E5">
+        <v>2.39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>